<commit_message>
Messaging - Message senders and recipients are now called 'MsgEndpoint's. If you want to send to a Person use CLASSIFY Person ISA MsgEndpoint.
This way, you can send messages to all sorts of endpoints, including Organizations, Persona, Departments, Orders, etc. etc.
</commit_message>
<xml_diff>
--- a/Messaging/MSG_Test.xlsx
+++ b/Messaging/MSG_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>[Persons]</t>
   </si>
@@ -153,50 +153,26 @@
     <t>cepAppUseProp</t>
   </si>
   <si>
-    <t>Johan</t>
-  </si>
-  <si>
-    <t>v.d. Geest</t>
-  </si>
-  <si>
-    <t>jvdgeest@gmail.com</t>
-  </si>
-  <si>
-    <t>Jorrit</t>
-  </si>
-  <si>
-    <t>de Boer</t>
-  </si>
-  <si>
-    <t>jorrit.deboer@tno.nl</t>
-  </si>
-  <si>
-    <t>Henk</t>
-  </si>
-  <si>
-    <t>Ensink</t>
-  </si>
-  <si>
-    <t>henk.ensink@tno.nl</t>
-  </si>
-  <si>
-    <t>Jeroen</t>
-  </si>
-  <si>
-    <t>Broekhuijsen</t>
-  </si>
-  <si>
-    <t>jeroen.broekhuijsen@tno.nl</t>
-  </si>
-  <si>
-    <t>+31653725229</t>
+    <t>type X to exclude</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>Firstname</t>
+  </si>
+  <si>
+    <t>Lastname</t>
+  </si>
+  <si>
+    <t>first.name@lastname.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -219,8 +195,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -232,8 +236,23 @@
         <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -241,21 +260,50 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Accent2" xfId="5" builtinId="33"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Input" xfId="3" builtinId="20"/>
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -556,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29:F29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,519 +624,532 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="str">
-        <f t="shared" ref="A3:A9" si="0">IF($B3="","",CONCATENATE($B3,"_",$C3))</f>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="A3" s="6" t="str">
+        <f>IF(OR($B3&lt;&gt;"",$C3=""),"",CONCATENATE($C3,"_",$D3))</f>
+        <v/>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="str">
+      <c r="A4" s="6" t="str">
+        <f t="shared" ref="A4:A10" si="0">IF(OR($B4&lt;&gt;"",$C4=""),"",CONCATENATE($C4,"_",$D4))</f>
+        <v/>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Michiel_Stornebrink</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="str">
+        <v>Firstname_Lastname</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Johan_v.d. Geest</v>
-      </c>
-      <c r="B5" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" t="s">
+        <v/>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="str">
+      <c r="D6"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Jorrit_de Boer</v>
-      </c>
-      <c r="B6" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="str">
+        <v/>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Henk_Ensink</v>
-      </c>
-      <c r="B7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" t="str">
+        <v/>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D8"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="str">
         <f t="shared" si="0"/>
-        <v>Jeroen_Broekhuijsen</v>
-      </c>
-      <c r="B8" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" t="str">
+        <v/>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B10" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10"/>
     </row>
     <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="1" t="str">
-        <f>$A11</f>
+      <c r="E12" s="1" t="str">
+        <f>$A12</f>
         <v>ContactEndpoint</v>
       </c>
-      <c r="F11" s="1" t="str">
-        <f>$A11</f>
+      <c r="F12" s="1" t="str">
+        <f>$A12</f>
         <v>ContactEndpoint</v>
       </c>
-      <c r="G11" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" t="str">
-        <f t="shared" ref="A12:A32" si="1">IF($B12="","",CONCATENATE("CEP_",ROW()))</f>
-        <v>CEP_12</v>
-      </c>
-      <c r="B12" t="str">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="str">
+        <f t="shared" ref="A13:A28" si="1">IF(OR($B13="",$B13=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v/>
+      </c>
+      <c r="B13" s="6" t="str">
         <f>$A$3</f>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C12" t="s">
+        <v/>
+      </c>
+      <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_13</v>
-      </c>
-      <c r="B13" t="str">
-        <f t="shared" ref="B13:B22" si="2">$A$3</f>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C13" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f t="shared" ref="B14:B23" si="2">$A$3</f>
+        <v/>
+      </c>
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_14</v>
-      </c>
-      <c r="B14" t="str">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B15" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C14" t="s">
-        <v>19</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="str">
-        <f>$A14</f>
-        <v>CEP_14</v>
-      </c>
-      <c r="F14" t="str">
-        <f>$A14</f>
-        <v>CEP_14</v>
-      </c>
-      <c r="G14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_15</v>
-      </c>
-      <c r="B15" t="str">
-        <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
+        <v/>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="str">
+        <f>$A15</f>
+        <v/>
+      </c>
+      <c r="F15" t="str">
+        <f>$A15</f>
+        <v/>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B16" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_16</v>
-      </c>
-      <c r="B16" t="str">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B17" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C16" t="s">
+        <v/>
+      </c>
+      <c r="C17" t="s">
         <v>28</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="D17" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_17</v>
-      </c>
-      <c r="B17" t="str">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B18" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C17" t="s">
+        <v/>
+      </c>
+      <c r="C18" t="s">
         <v>29</v>
       </c>
-      <c r="D17" s="3" t="s">
+      <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_18</v>
-      </c>
-      <c r="B18" t="str">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B19" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C18" t="s">
+        <v/>
+      </c>
+      <c r="C19" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_19</v>
-      </c>
-      <c r="B19" t="str">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B20" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C19" t="s">
+        <v/>
+      </c>
+      <c r="C20" t="s">
         <v>32</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D20" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_20</v>
-      </c>
-      <c r="B20" t="str">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B21" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C20" t="s">
+        <v/>
+      </c>
+      <c r="C21" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="D21" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_21</v>
-      </c>
-      <c r="B21" t="str">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B22" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C21" t="s">
+        <v/>
+      </c>
+      <c r="C22" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_22</v>
-      </c>
-      <c r="B22" t="str">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B23" s="6" t="str">
         <f t="shared" si="2"/>
-        <v>Rieks_Joosten</v>
-      </c>
-      <c r="C22" t="s">
+        <v/>
+      </c>
+      <c r="C23" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G22" t="s">
+      <c r="G23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-    </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_24</v>
-      </c>
-      <c r="B24" t="str">
+      <c r="A24" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B25" s="6" t="str">
         <f>$A$4</f>
-        <v>Michiel_Stornebrink</v>
-      </c>
-      <c r="C24" t="s">
+        <v/>
+      </c>
+      <c r="C25" t="s">
         <v>10</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E24" t="str">
-        <f>$A24</f>
-        <v>CEP_24</v>
-      </c>
-      <c r="F24" t="str">
-        <f>$A24</f>
-        <v>CEP_24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_25</v>
-      </c>
-      <c r="B25" t="str">
-        <f t="shared" ref="B25:B26" si="3">$A$4</f>
-        <v>Michiel_Stornebrink</v>
-      </c>
-      <c r="C25" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>22</v>
       </c>
       <c r="E25" t="str">
         <f>$A25</f>
-        <v>CEP_25</v>
+        <v/>
       </c>
       <c r="F25" t="str">
         <f>$A25</f>
-        <v>CEP_25</v>
+        <v/>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_26</v>
-      </c>
-      <c r="B26" t="str">
+      <c r="A26" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B26" s="6" t="str">
+        <f t="shared" ref="B26:B27" si="3">$A$4</f>
+        <v/>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="str">
+        <f>$A26</f>
+        <v/>
+      </c>
+      <c r="F26" t="str">
+        <f>$A26</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B27" s="6" t="str">
         <f t="shared" si="3"/>
-        <v>Michiel_Stornebrink</v>
-      </c>
-      <c r="C26" t="s">
+        <v/>
+      </c>
+      <c r="C27" t="s">
         <v>39</v>
       </c>
-      <c r="D26" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="D27" s="4"/>
-    </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_28</v>
-      </c>
-      <c r="B28" t="str">
+      <c r="A28" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="str">
+        <f>IF(OR($B29="",$B29=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v>CEP_29</v>
+      </c>
+      <c r="B29" s="6" t="str">
         <f>$A$5</f>
-        <v>Johan_v.d. Geest</v>
-      </c>
-      <c r="C28" t="s">
-        <v>19</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_29</v>
-      </c>
-      <c r="B29" t="str">
-        <f>$A$6</f>
-        <v>Jorrit_de Boer</v>
+        <v>Firstname_Lastname</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="E29" t="str">
-        <f>$A29</f>
-        <v>CEP_29</v>
-      </c>
-      <c r="F29" t="str">
-        <f>$A29</f>
-        <v>CEP_29</v>
+        <v>49</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_30</v>
-      </c>
-      <c r="B30" t="str">
+      <c r="A30" s="6" t="str">
+        <f t="shared" ref="A30:A34" si="4">IF(OR($B30="",$B30=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v/>
+      </c>
+      <c r="B30" s="6" t="str">
+        <f>$A$6</f>
+        <v/>
+      </c>
+      <c r="D30" s="4"/>
+      <c r="E30" t="str">
+        <f>$A30</f>
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <f>$A30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B31" s="6" t="str">
+        <f>$A$8</f>
+        <v/>
+      </c>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B32" s="6" t="str">
+        <f>$A$9</f>
+        <v/>
+      </c>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B33" s="6" t="str">
+        <f>$A$9</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B34" s="6" t="str">
         <f>$A$7</f>
-        <v>Henk_Ensink</v>
-      </c>
-      <c r="C30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_31</v>
-      </c>
-      <c r="B31" t="str">
-        <f>$A$8</f>
-        <v>Jeroen_Broekhuijsen</v>
-      </c>
-      <c r="C31" t="s">
-        <v>19</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_32</v>
-      </c>
-      <c r="B32" t="str">
-        <f>$A$8</f>
-        <v>Jeroen_Broekhuijsen</v>
-      </c>
-      <c r="C32" t="s">
-        <v>33</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>57</v>
+        <v/>
+      </c>
+      <c r="D34" s="5"/>
+      <c r="E34" t="str">
+        <f>$A34</f>
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <f>$A34</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D14" r:id="rId1"/>
-    <hyperlink ref="D15" r:id="rId2"/>
-    <hyperlink ref="D25" r:id="rId3"/>
-    <hyperlink ref="D28" r:id="rId4"/>
-    <hyperlink ref="D30" r:id="rId5"/>
-    <hyperlink ref="D29" r:id="rId6"/>
-    <hyperlink ref="D31" r:id="rId7"/>
+    <hyperlink ref="D15" r:id="rId1"/>
+    <hyperlink ref="D16" r:id="rId2"/>
+    <hyperlink ref="D26" r:id="rId3"/>
+    <hyperlink ref="D29" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
SIAM and Messaging updates that should take effect when #228 is resolved
</commit_message>
<xml_diff>
--- a/Messaging/MSG_Test.xlsx
+++ b/Messaging/MSG_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="63">
   <si>
     <t>[Persons]</t>
   </si>
@@ -48,6 +48,12 @@
     <t>cepNote</t>
   </si>
   <si>
+    <t>Pushover</t>
+  </si>
+  <si>
+    <t>ufoaKLBxhPxdiECpxtxhdjqdSMyfDD</t>
+  </si>
+  <si>
     <t>Rieks</t>
   </si>
   <si>
@@ -60,12 +66,24 @@
     <t>Stornebrink</t>
   </si>
   <si>
+    <t>uaFR8QKy4S4Bs8r3KNekMB3xmdnaox</t>
+  </si>
+  <si>
+    <t>Pushalot</t>
+  </si>
+  <si>
+    <t>7872fd42684b4f81b908c80618814b18</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
     <t>rieks.joosten@tno.nl</t>
   </si>
   <si>
+    <t>rj2002060@outlook.com</t>
+  </si>
+  <si>
     <t>michiel.stornebrink@tno.nl</t>
   </si>
   <si>
@@ -84,15 +102,39 @@
     <t>cepAddress</t>
   </si>
   <si>
+    <t>Skype</t>
+  </si>
+  <si>
     <t>Phone</t>
   </si>
   <si>
+    <t>r1ek5j</t>
+  </si>
+  <si>
+    <t>Fax</t>
+  </si>
+  <si>
+    <t>Linkedin</t>
+  </si>
+  <si>
     <t>SMS</t>
   </si>
   <si>
+    <t>Twitter</t>
+  </si>
+  <si>
+    <t>RJ_tno</t>
+  </si>
+  <si>
     <t>+31622901317</t>
   </si>
   <si>
+    <t>+3188667744</t>
+  </si>
+  <si>
+    <t>https://nl.linkedin.com/in/rjoosten</t>
+  </si>
+  <si>
     <t>Mail</t>
   </si>
   <si>
@@ -102,29 +144,74 @@
     <t>Mail die hier naartoe gestuurd wordt, lees ik doorgaans binnen een dag.</t>
   </si>
   <si>
+    <t>Ik heb hem wel, maar gebruik hetm eigenlijk nooit</t>
+  </si>
+  <si>
     <t>cepAppIsValid</t>
   </si>
   <si>
     <t>cepAppUseProp</t>
   </si>
   <si>
+    <t>Johan</t>
+  </si>
+  <si>
+    <t>v.d. Geest</t>
+  </si>
+  <si>
+    <t>jvdgeest@gmail.com</t>
+  </si>
+  <si>
     <t>Jorrit</t>
   </si>
   <si>
     <t>de Boer</t>
   </si>
   <si>
+    <t>jorrit.deboer@tno.nl</t>
+  </si>
+  <si>
+    <t>henk.ensink@tno.nl</t>
+  </si>
+  <si>
+    <t>jeroen.broekhuijsen@tno.nl</t>
+  </si>
+  <si>
+    <t>+31653725229</t>
+  </si>
+  <si>
+    <t>henk.wiersema@tno.nl</t>
+  </si>
+  <si>
     <t>type X to exclude</t>
   </si>
   <si>
     <t>x</t>
+  </si>
+  <si>
+    <t>Stef</t>
+  </si>
+  <si>
+    <t>Han</t>
+  </si>
+  <si>
+    <t>Han.Joosten@ordina.nl</t>
+  </si>
+  <si>
+    <t>han.joosten.han@gmail.com</t>
+  </si>
+  <si>
+    <t>stef.joosten@ou.nl</t>
+  </si>
+  <si>
+    <t>stef.joosten@ordina.nl</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -146,6 +233,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -226,21 +319,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="4"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="4"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="3" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="5" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -549,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -580,8 +674,8 @@
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>32</v>
+      <c r="B2" s="8" t="s">
+        <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -591,241 +685,637 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="5" t="str">
+      <c r="A3" s="6" t="str">
         <f>IF(OR($B3&lt;&gt;"",$C3=""),"",CONCATENATE($C3," ",$D3))</f>
         <v>Rieks Joosten</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="7"/>
       <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="str">
+        <f t="shared" ref="A4:A10" si="0">IF(OR($B4&lt;&gt;"",$C4=""),"",CONCATENATE($C4," ",$D4))</f>
+        <v>Michiel Stornebrink</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Stef Joosten</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v>Han Joosten</v>
+      </c>
+      <c r="B8" s="7"/>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+      <c r="B10" s="7"/>
+      <c r="D10"/>
+    </row>
+    <row r="11" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="1" t="str">
+        <f>$A12</f>
+        <v>ContactEndpoint</v>
+      </c>
+      <c r="F12" s="1" t="str">
+        <f>$A12</f>
+        <v>ContactEndpoint</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="6" t="str">
+        <f t="shared" ref="A13:A28" si="1">IF(OR($B13="",$B13=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v>CEP_13</v>
+      </c>
+      <c r="B13" s="6" t="str">
+        <f>$A$3</f>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C13" t="s">
         <v>10</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D13" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="str">
-        <f t="shared" ref="A4:A6" si="0">IF(OR($B4&lt;&gt;"",$C4=""),"",CONCATENATE($C4," ",$D4))</f>
-        <v>Michiel Stornebrink</v>
-      </c>
-      <c r="B4" s="6"/>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="str">
-        <f t="shared" si="0"/>
-        <v/>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6"/>
-    </row>
-    <row r="7" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="1" t="s">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_14</v>
+      </c>
+      <c r="B14" s="6" t="str">
+        <f t="shared" ref="B14:B23" si="2">$A$3</f>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C14" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="1" t="str">
-        <f>$A8</f>
-        <v>ContactEndpoint</v>
-      </c>
-      <c r="F8" s="1" t="str">
-        <f>$A8</f>
-        <v>ContactEndpoint</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="str">
-        <f t="shared" ref="A9:A16" si="1">IF(OR($B9="",$B9=0),"",CONCATENATE("CEP_",ROW()))</f>
-        <v>CEP_9</v>
-      </c>
-      <c r="B9" s="5" t="str">
-        <f t="shared" ref="B9:B12" si="2">$A$3</f>
-        <v>Rieks Joosten</v>
-      </c>
-      <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" t="str">
-        <f>$A9</f>
-        <v>CEP_9</v>
-      </c>
-      <c r="F9" t="str">
-        <f>$A9</f>
-        <v>CEP_9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_10</v>
-      </c>
-      <c r="B10" s="5" t="str">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_15</v>
+      </c>
+      <c r="B15" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Rieks Joosten</v>
       </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_11</v>
-      </c>
-      <c r="B11" s="5" t="str">
+      <c r="C15" t="s">
+        <v>19</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" t="str">
+        <f>$A15</f>
+        <v>CEP_15</v>
+      </c>
+      <c r="F15" t="str">
+        <f>$A15</f>
+        <v>CEP_15</v>
+      </c>
+      <c r="G15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_16</v>
+      </c>
+      <c r="B16" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Rieks Joosten</v>
       </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_12</v>
-      </c>
-      <c r="B12" s="5" t="str">
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_17</v>
+      </c>
+      <c r="B17" s="6" t="str">
         <f t="shared" si="2"/>
         <v>Rieks Joosten</v>
       </c>
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_14</v>
-      </c>
-      <c r="B14" s="5" t="str">
-        <f t="shared" ref="B14:B15" si="3">$A$4</f>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_18</v>
+      </c>
+      <c r="B18" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_19</v>
+      </c>
+      <c r="B19" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C19" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_20</v>
+      </c>
+      <c r="B20" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_21</v>
+      </c>
+      <c r="B21" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_22</v>
+      </c>
+      <c r="B22" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_23</v>
+      </c>
+      <c r="B23" s="6" t="str">
+        <f t="shared" si="2"/>
+        <v>Rieks Joosten</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B24" s="6"/>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_25</v>
+      </c>
+      <c r="B25" s="6" t="str">
+        <f>$A$4</f>
         <v>Michiel Stornebrink</v>
       </c>
-      <c r="C14" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="4" t="s">
+      <c r="C25" t="s">
+        <v>10</v>
+      </c>
+      <c r="D25" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E14" t="str">
-        <f>$A14</f>
-        <v>CEP_14</v>
-      </c>
-      <c r="F14" t="str">
-        <f>$A14</f>
-        <v>CEP_14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v>CEP_15</v>
-      </c>
-      <c r="B15" s="5" t="str">
+      <c r="E25" t="str">
+        <f>$A25</f>
+        <v>CEP_25</v>
+      </c>
+      <c r="F25" t="str">
+        <f>$A25</f>
+        <v>CEP_25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_26</v>
+      </c>
+      <c r="B26" s="6" t="str">
+        <f t="shared" ref="B26:B27" si="3">$A$4</f>
+        <v>Michiel Stornebrink</v>
+      </c>
+      <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E26" t="str">
+        <f>$A26</f>
+        <v>CEP_26</v>
+      </c>
+      <c r="F26" t="str">
+        <f>$A26</f>
+        <v>CEP_26</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v>CEP_27</v>
+      </c>
+      <c r="B27" s="6" t="str">
         <f t="shared" si="3"/>
         <v>Michiel Stornebrink</v>
       </c>
-      <c r="C15" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="str">
-        <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="B16" s="5"/>
-      <c r="D16" s="4"/>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" s="6" t="str">
+        <f t="shared" si="1"/>
+        <v/>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" s="6" t="str">
+        <f>IF(OR($B29="",$B29=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v/>
+      </c>
+      <c r="B29" s="6" t="str">
+        <f>$A$5</f>
+        <v/>
+      </c>
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" s="6" t="str">
+        <f t="shared" ref="A30:A39" si="4">IF(OR($B30="",$B30=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v/>
+      </c>
+      <c r="B30" s="6" t="str">
+        <f>$A$6</f>
+        <v/>
+      </c>
+      <c r="C30" t="s">
+        <v>19</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="E30" t="str">
+        <f>$A30</f>
+        <v/>
+      </c>
+      <c r="F30" t="str">
+        <f>$A30</f>
+        <v/>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" s="6" t="str">
+        <f>IF(OR($B31="",$B31=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v/>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" t="s">
+        <v>19</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" t="s">
+        <v>19</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" t="s">
+        <v>33</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" t="s">
+        <v>19</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="E34" t="str">
+        <f>$A34</f>
+        <v/>
+      </c>
+      <c r="F34" t="str">
+        <f>$A34</f>
+        <v/>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="B35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>CEP_36</v>
+      </c>
+      <c r="B36" s="6" t="str">
+        <f t="shared" ref="B36:B37" si="5">$A$7</f>
+        <v>Stef Joosten</v>
+      </c>
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" ref="E36:F39" si="6">$A36</f>
+        <v>CEP_36</v>
+      </c>
+      <c r="F36" t="str">
+        <f t="shared" si="6"/>
+        <v>CEP_36</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="6" t="str">
+        <f>IF(OR($B37="",$B37=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v>CEP_37</v>
+      </c>
+      <c r="B37" s="6" t="str">
+        <f t="shared" si="5"/>
+        <v>Stef Joosten</v>
+      </c>
+      <c r="C37" t="s">
+        <v>19</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="6"/>
+        <v>CEP_37</v>
+      </c>
+      <c r="F37" t="str">
+        <f t="shared" si="6"/>
+        <v>CEP_37</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="6" t="str">
+        <f>IF(OR($B38="",$B38=0),"",CONCATENATE("CEP_",ROW()))</f>
+        <v>CEP_38</v>
+      </c>
+      <c r="B38" s="6" t="str">
+        <f>$A$8</f>
+        <v>Han Joosten</v>
+      </c>
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="6"/>
+        <v>CEP_38</v>
+      </c>
+      <c r="F38" t="str">
+        <f t="shared" si="6"/>
+        <v>CEP_38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="6" t="str">
+        <f t="shared" si="4"/>
+        <v>CEP_39</v>
+      </c>
+      <c r="B39" s="6" t="str">
+        <f>$A$8</f>
+        <v>Han Joosten</v>
+      </c>
+      <c r="C39" t="s">
+        <v>19</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E39" t="str">
+        <f>$A39</f>
+        <v>CEP_39</v>
+      </c>
+      <c r="F39" t="str">
+        <f t="shared" si="6"/>
+        <v>CEP_39</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
-    <hyperlink ref="D14" r:id="rId2"/>
+    <hyperlink ref="D15" r:id="rId1"/>
+    <hyperlink ref="D16" r:id="rId2"/>
+    <hyperlink ref="D26" r:id="rId3"/>
+    <hyperlink ref="D29" r:id="rId4"/>
+    <hyperlink ref="D31" r:id="rId5"/>
+    <hyperlink ref="D30" r:id="rId6"/>
+    <hyperlink ref="D32" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 

</xml_diff>